<commit_message>
Completed Connecting Excel data to Webops Class
</commit_message>
<xml_diff>
--- a/Data/Info/MasterList.xlsx
+++ b/Data/Info/MasterList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice\gitRepo\Data\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A7D4E8-E8FB-4EB6-B834-6C226FDDEA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE182A77-F09D-42D4-BC7F-409DA811BBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32685" yWindow="615" windowWidth="17310" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Keywords</t>
   </si>
@@ -41,16 +41,58 @@
     <t>Experience</t>
   </si>
   <si>
-    <t>Sofware Developer job; Java; Python</t>
-  </si>
-  <si>
-    <t>data scientist job; SQL; Python</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://www.google.com/</t>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>999-999-9999</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>testCity</t>
+  </si>
+  <si>
+    <t>exactPhrase</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>Java; Python</t>
+  </si>
+  <si>
+    <t>developer engineer</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>analysist scientist</t>
+  </si>
+  <si>
+    <t>SQL; Python</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
   </si>
 </sst>
 </file>
@@ -94,10 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,10 +441,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -413,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61791F76-3F62-4D8B-A56F-EDA96CE6FC07}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,18 +508,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -457,10 +546,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6426FE-A1FC-48DA-AB40-4B493E53D3F8}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,18 +567,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>